<commit_message>
update by SCJ 更新
</commit_message>
<xml_diff>
--- a/Amazon/AmazonJP/Htmls/Htmls.xlsx
+++ b/Amazon/AmazonJP/Htmls/Htmls.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\test5\PythonProject\Amazon\AmazonJP\Htmls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18465" windowHeight="9510"/>
+    <workbookView windowWidth="28560" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon" sheetId="1" r:id="rId1"/>
@@ -19,16 +14,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1">
   <si>
-    <t>https://www.amazon.co.jp/%E3%82%A8%E3%83%8C%E3%83%86%E3%82%A3%E3%83%BC-%E3%82%AB%E3%83%BC%E3%83%88%E3%83%AA%E3%83%83%E3%82%B8%E5%BC%8F%E3%82%AB%E3%83%83%E3%82%BF%E3%83%BC-6%E9%80%A3%E7%99%BA%E3%82%BF%E3%82%A4%E3%83%97-%E3%83%96%E3%83%A9%E3%83%83%E3%82%AF-L-700RP-BK/dp/B004MXKHR2/ref=sr_1_14?s=office-products&amp;rps=1&amp;ie=UTF8&amp;qid=1479035637&amp;sr=1-14&amp;keywords=%E6%97%A5%E6%9C%AC%E8%A3%BD</t>
+    <t>https://www.amazon.co.jp/gp/product/B00U5NQKZ6/ref=s9_acsd_ri_bw_rw_r0_p2_t_w?pf_rd_m=AN1VRQENFRJN5&amp;pf_rd_s=merchandised-search-10&amp;pf_rd_r=XQ389905HSG7YA4WNGPN&amp;pf_rd_r=XQ389905HSG7YA4WNGPN&amp;pf_rd_t=101&amp;pf_rd_p=d533e1c7-a774-4ae9-9ef1-75fe61352674&amp;pf_rd_p=d533e1c7-a774-4ae9-9ef1-75fe61352674&amp;pf_rd_i=2547227051</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,21 +45,352 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -66,9 +398,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -76,24 +650,63 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规 2" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -383,14 +996,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="24.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
@@ -398,14 +1012,14 @@
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>